<commit_message>
Asignación de autores mat 9 tema 4
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion04/Escaleta MA_09_04_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion04/Escaleta MA_09_04_CO.xlsx
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="256">
   <si>
     <t>Asignatura</t>
   </si>
@@ -527,9 +527,6 @@
     <t>Interactivo que presenta el concepto de fracción, sus notaciones y representaciones</t>
   </si>
   <si>
-    <t>MODELACIÓN</t>
-  </si>
-  <si>
     <t xml:space="preserve">NUEVO </t>
   </si>
   <si>
@@ -542,18 +539,12 @@
     <t>Actividad para reconocer las formas algebraicas de los trozos de una función</t>
   </si>
   <si>
-    <t>EJERCITACIÓN</t>
-  </si>
-  <si>
     <t>ACTIVIDAD</t>
   </si>
   <si>
     <t>Actividad para reconocer cuando una representación determina una función</t>
   </si>
   <si>
-    <t>RAZONAMIENTO</t>
-  </si>
-  <si>
     <t xml:space="preserve">APROVECHADO </t>
   </si>
   <si>
@@ -563,9 +554,6 @@
     <t>Actividad para reconocer funciones representadas en un diagrama sagital</t>
   </si>
   <si>
-    <t>RESOLUCIÓN DE PROBLEMAS</t>
-  </si>
-  <si>
     <t>Interactivo para mostrar la gráfica de una función y la tabla de valores que la representa</t>
   </si>
   <si>
@@ -801,6 +789,9 @@
   </si>
   <si>
     <t>InActividad que presenta ejemplos de problemas que se solucionan a partir de modelos funcionales</t>
+  </si>
+  <si>
+    <t>Clara</t>
   </si>
 </sst>
 </file>
@@ -855,7 +846,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -940,6 +931,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -968,7 +965,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1050,19 +1047,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1085,6 +1073,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1390,11 +1390,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U285"/>
+  <dimension ref="A1:V285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="A37:XFD37"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V25" sqref="V25:V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,97 +1422,97 @@
     <col min="22" max="16384" width="11.42578125" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="21" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:22" s="21" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="39"/>
-      <c r="O1" s="29" t="s">
+      <c r="N1" s="36"/>
+      <c r="O1" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="Q1" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="32" t="s">
+      <c r="R1" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="30" t="s">
+      <c r="S1" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="T1" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="30" t="s">
+      <c r="U1" s="38" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="36"/>
+    <row r="2" spans="1:22" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="33"/>
       <c r="M2" s="8" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="30"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="38"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -1540,38 +1540,41 @@
         <v>166</v>
       </c>
       <c r="K3" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>55</v>
       </c>
       <c r="N3" s="7"/>
       <c r="O3" s="25" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="P3" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q3" s="10">
         <v>6</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="U3" s="10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="V3" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1593,23 +1596,23 @@
         <v>2</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="J4" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="K4" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>171</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>173</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="7" t="s">
         <v>33</v>
       </c>
       <c r="O4" s="25" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="P4" s="26" t="s">
         <v>165</v>
@@ -1618,19 +1621,22 @@
         <v>6</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="U4" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="V4" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1652,23 +1658,23 @@
         <v>3</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7" t="s">
         <v>37</v>
       </c>
       <c r="O5" s="27" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="P5" s="26" t="s">
         <v>165</v>
@@ -1677,19 +1683,22 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="T5" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="S5" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="T5" s="12" t="s">
-        <v>209</v>
-      </c>
       <c r="U5" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="V5" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1711,11 +1720,11 @@
         <v>4</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="J6" s="24"/>
       <c r="K6" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="7"/>
@@ -1723,7 +1732,7 @@
       <c r="O6" s="27"/>
       <c r="P6" s="26"/>
       <c r="Q6" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R6" s="11" t="s">
         <v>129</v>
@@ -1732,13 +1741,13 @@
         <v>130</v>
       </c>
       <c r="T6" s="15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="U6" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -1762,10 +1771,10 @@
         <v>5</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="5"/>
@@ -1776,7 +1785,7 @@
       <c r="O7" s="25"/>
       <c r="P7" s="26"/>
       <c r="Q7" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R7" s="11" t="s">
         <v>129</v>
@@ -1791,7 +1800,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1813,23 +1822,23 @@
         <v>6</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="7" t="s">
         <v>39</v>
       </c>
       <c r="O8" s="25" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="P8" s="26" t="s">
         <v>165</v>
@@ -1838,19 +1847,22 @@
         <v>6</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="V8" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1875,20 +1887,20 @@
         <v>165</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K9" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="M9" s="7" t="s">
         <v>54</v>
       </c>
       <c r="N9" s="7"/>
       <c r="O9" s="25" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="P9" s="26" t="s">
         <v>165</v>
@@ -1897,19 +1909,22 @@
         <v>6</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="V9" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1931,23 +1946,23 @@
         <v>8</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M10" s="7" t="s">
         <v>53</v>
       </c>
       <c r="N10" s="7"/>
       <c r="O10" s="25" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="P10" s="26" t="s">
         <v>165</v>
@@ -1956,19 +1971,22 @@
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="V10" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -1992,7 +2010,7 @@
         <v>9</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J11" s="24"/>
       <c r="K11" s="6"/>
@@ -2002,7 +2020,7 @@
       <c r="O11" s="25"/>
       <c r="P11" s="26"/>
       <c r="Q11" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R11" s="11" t="s">
         <v>129</v>
@@ -2011,13 +2029,13 @@
         <v>130</v>
       </c>
       <c r="T11" s="15" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="U11" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -2039,10 +2057,10 @@
         <v>10</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="5"/>
@@ -2051,7 +2069,7 @@
       <c r="O12" s="25"/>
       <c r="P12" s="26"/>
       <c r="Q12" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R12" s="11" t="s">
         <v>129</v>
@@ -2060,13 +2078,13 @@
         <v>130</v>
       </c>
       <c r="T12" s="15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="U12" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -2088,7 +2106,7 @@
         <v>11</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="6"/>
@@ -2098,7 +2116,7 @@
       <c r="O13" s="25"/>
       <c r="P13" s="26"/>
       <c r="Q13" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R13" s="11" t="s">
         <v>129</v>
@@ -2113,7 +2131,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -2135,23 +2153,23 @@
         <v>12</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M14" s="7"/>
       <c r="N14" s="7" t="s">
         <v>40</v>
       </c>
       <c r="O14" s="25" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="P14" s="26" t="s">
         <v>165</v>
@@ -2160,19 +2178,22 @@
         <v>6</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="V14" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -2196,13 +2217,13 @@
         <v>13</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L15" s="5"/>
       <c r="M15" s="7"/>
@@ -2210,7 +2231,7 @@
       <c r="O15" s="25"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R15" s="11" t="s">
         <v>129</v>
@@ -2219,13 +2240,13 @@
         <v>130</v>
       </c>
       <c r="T15" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="U15" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -2247,44 +2268,44 @@
         <v>14</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M16" s="7"/>
       <c r="N16" s="7" t="s">
         <v>29</v>
       </c>
       <c r="O16" s="25" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="P16" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q16" s="10">
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -2306,16 +2327,16 @@
         <v>15</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
@@ -2324,7 +2345,7 @@
         <v>165</v>
       </c>
       <c r="Q17" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R17" s="11" t="s">
         <v>129</v>
@@ -2333,13 +2354,13 @@
         <v>130</v>
       </c>
       <c r="T17" s="15" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="U17" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -2361,10 +2382,10 @@
         <v>16</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="J18" s="24" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="5"/>
@@ -2373,7 +2394,7 @@
       <c r="O18" s="25"/>
       <c r="P18" s="26"/>
       <c r="Q18" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R18" s="11" t="s">
         <v>129</v>
@@ -2388,7 +2409,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -2415,20 +2436,20 @@
         <v>165</v>
       </c>
       <c r="J19" s="24" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K19" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="L19" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="M19" s="7" t="s">
         <v>54</v>
       </c>
       <c r="N19" s="7"/>
       <c r="O19" s="25" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="P19" s="26" t="s">
         <v>165</v>
@@ -2437,19 +2458,19 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
@@ -2471,27 +2492,27 @@
         <v>18</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
       <c r="O20" s="25" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="P20" s="26" t="s">
         <v>165</v>
       </c>
       <c r="Q20" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R20" s="11" t="s">
         <v>129</v>
@@ -2500,13 +2521,13 @@
         <v>130</v>
       </c>
       <c r="T20" s="15" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="U20" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
@@ -2528,27 +2549,27 @@
         <v>19</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J21" s="24" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
       <c r="O21" s="25" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="P21" s="26" t="s">
         <v>165</v>
       </c>
       <c r="Q21" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R21" s="11" t="s">
         <v>129</v>
@@ -2563,7 +2584,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
@@ -2585,23 +2606,23 @@
         <v>20</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J22" s="24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M22" s="7"/>
       <c r="N22" s="7" t="s">
         <v>28</v>
       </c>
       <c r="O22" s="25" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="P22" s="26" t="s">
         <v>165</v>
@@ -2610,19 +2631,22 @@
         <v>6</v>
       </c>
       <c r="R22" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="U22" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="V22" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
@@ -2644,7 +2668,7 @@
         <v>21</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J23" s="24"/>
       <c r="K23" s="6"/>
@@ -2654,7 +2678,7 @@
       <c r="O23" s="25"/>
       <c r="P23" s="26"/>
       <c r="Q23" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R23" s="11" t="s">
         <v>129</v>
@@ -2663,13 +2687,13 @@
         <v>130</v>
       </c>
       <c r="T23" s="15" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="U23" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -2693,7 +2717,7 @@
         <v>22</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J24" s="24"/>
       <c r="K24" s="6"/>
@@ -2703,7 +2727,7 @@
       <c r="O24" s="25"/>
       <c r="P24" s="26"/>
       <c r="Q24" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R24" s="11" t="s">
         <v>129</v>
@@ -2718,7 +2742,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
@@ -2729,7 +2753,7 @@
         <v>123</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="14"/>
@@ -2743,41 +2767,44 @@
         <v>165</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M25" s="7" t="s">
         <v>56</v>
       </c>
       <c r="N25" s="7"/>
       <c r="O25" s="27" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="P25" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q25" s="10">
         <v>6</v>
       </c>
       <c r="R25" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="S25" s="10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="T25" s="12" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="U25" s="10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="V25" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -2788,7 +2815,7 @@
         <v>123</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="14"/>
@@ -2799,23 +2826,23 @@
         <v>24</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M26" s="7"/>
       <c r="N26" s="7" t="s">
         <v>29</v>
       </c>
       <c r="O26" s="25" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="P26" s="26" t="s">
         <v>165</v>
@@ -2824,19 +2851,22 @@
         <v>6</v>
       </c>
       <c r="R26" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="S26" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="T26" s="12" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="V26" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
@@ -2847,23 +2877,25 @@
         <v>123</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="14"/>
       <c r="G27" s="22" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H27" s="23">
         <v>25</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>252</v>
-      </c>
-      <c r="K27" s="6"/>
+        <v>248</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>167</v>
+      </c>
       <c r="L27" s="5"/>
       <c r="M27" s="7"/>
       <c r="N27" s="7" t="s">
@@ -2875,19 +2907,22 @@
         <v>6</v>
       </c>
       <c r="R27" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="S27" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="T27" s="12" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="U27" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="V27" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>15</v>
       </c>
@@ -2912,41 +2947,44 @@
         <v>165</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="K28" s="6" t="s">
         <v>167</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M28" s="7" t="s">
         <v>59</v>
       </c>
       <c r="N28" s="7"/>
       <c r="O28" s="25" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="P28" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q28" s="10">
         <v>6</v>
       </c>
       <c r="R28" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="T28" s="12" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="V28" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>15</v>
       </c>
@@ -2968,23 +3006,23 @@
         <v>27</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="M29" s="7"/>
       <c r="N29" s="7" t="s">
         <v>39</v>
       </c>
       <c r="O29" s="25" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="P29" s="26" t="s">
         <v>165</v>
@@ -2993,19 +3031,22 @@
         <v>6</v>
       </c>
       <c r="R29" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="S29" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="T29" s="12" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="U29" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="V29" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>15</v>
       </c>
@@ -3029,10 +3070,12 @@
         <v>28</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J30" s="24"/>
-      <c r="K30" s="6"/>
+      <c r="K30" s="6" t="s">
+        <v>167</v>
+      </c>
       <c r="L30" s="5"/>
       <c r="M30" s="7"/>
       <c r="N30" s="7" t="s">
@@ -3044,19 +3087,22 @@
         <v>6</v>
       </c>
       <c r="R30" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="S30" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="T30" s="12" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="U30" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="V30" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
@@ -3067,7 +3113,7 @@
         <v>123</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="14"/>
@@ -3078,7 +3124,7 @@
         <v>29</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J31" s="24"/>
       <c r="K31" s="6"/>
@@ -3088,7 +3134,7 @@
       <c r="O31" s="25"/>
       <c r="P31" s="26"/>
       <c r="Q31" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R31" s="11" t="s">
         <v>129</v>
@@ -3097,13 +3143,16 @@
         <v>130</v>
       </c>
       <c r="T31" s="15" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="U31" s="10" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V31" s="41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>15</v>
       </c>
@@ -3114,7 +3163,7 @@
         <v>123</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="14"/>
@@ -3125,23 +3174,23 @@
         <v>30</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J32" s="24" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="L32" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M32" s="7" t="s">
         <v>63</v>
       </c>
       <c r="N32" s="7"/>
       <c r="O32" s="25" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="P32" s="26" t="s">
         <v>165</v>
@@ -3150,16 +3199,19 @@
         <v>6</v>
       </c>
       <c r="R32" s="11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="S32" s="10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="T32" s="12" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="U32" s="10" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="V32" s="41" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3173,7 +3225,7 @@
         <v>123</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E33" s="13"/>
       <c r="F33" s="14"/>
@@ -3184,10 +3236,10 @@
         <v>31</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J33" s="24" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="K33" s="6"/>
       <c r="L33" s="5"/>
@@ -3196,7 +3248,7 @@
       <c r="O33" s="25"/>
       <c r="P33" s="26"/>
       <c r="Q33" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R33" s="11" t="s">
         <v>129</v>
@@ -3205,7 +3257,7 @@
         <v>130</v>
       </c>
       <c r="T33" s="15" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="U33" s="10" t="s">
         <v>132</v>
@@ -3222,7 +3274,7 @@
         <v>123</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="14"/>
@@ -3233,10 +3285,10 @@
         <v>32</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J34" s="24" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="K34" s="6"/>
       <c r="L34" s="5"/>
@@ -3245,7 +3297,7 @@
       <c r="O34" s="25"/>
       <c r="P34" s="26"/>
       <c r="Q34" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R34" s="11" t="s">
         <v>129</v>
@@ -3271,7 +3323,7 @@
         <v>123</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E35" s="13"/>
       <c r="F35" s="14"/>
@@ -3282,12 +3334,14 @@
         <v>33</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J35" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="K35" s="6"/>
+        <v>193</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>167</v>
+      </c>
       <c r="L35" s="5"/>
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
@@ -3310,7 +3364,7 @@
         <v>123</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E36" s="13"/>
       <c r="F36" s="14"/>
@@ -3321,12 +3375,14 @@
         <v>34</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J36" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="K36" s="6"/>
+        <v>194</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>167</v>
+      </c>
       <c r="L36" s="5"/>
       <c r="M36" s="7"/>
       <c r="N36" s="7" t="s">
@@ -3338,16 +3394,16 @@
         <v>6</v>
       </c>
       <c r="R36" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="S36" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="T36" s="12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="U36" s="10" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3361,7 +3417,7 @@
         <v>123</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E37" s="13"/>
       <c r="F37" s="14"/>
@@ -3370,7 +3426,7 @@
         <v>35</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J37" s="24"/>
       <c r="K37" s="6"/>
@@ -3380,7 +3436,7 @@
       <c r="O37" s="25"/>
       <c r="P37" s="26"/>
       <c r="Q37" s="10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R37" s="11" t="s">
         <v>129</v>
@@ -3389,7 +3445,7 @@
         <v>130</v>
       </c>
       <c r="T37" s="15" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="U37" s="10" t="s">
         <v>132</v>
@@ -4529,6 +4585,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4543,18 +4605,9 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K23:K37">
-      <formula1>$H$62:$H$66</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K22 L30:L37 L23:L24">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K37 L30:L37 L23:L24">
       <formula1>$C$57:$G$57</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L25:L29 L3:L22">

</xml_diff>

<commit_message>
Encargo de recursos mat 9 tema 4
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion04/Escaleta MA_09_04_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion04/Escaleta MA_09_04_CO.xlsx
@@ -846,7 +846,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -937,6 +937,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -965,7 +977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1047,10 +1059,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1074,16 +1098,22 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1392,9 +1422,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V25" sqref="V25:V32"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,8 +1442,8 @@
     <col min="11" max="11" width="13.28515625" style="20" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" style="20" customWidth="1"/>
     <col min="13" max="14" width="9.28515625" style="20" customWidth="1"/>
-    <col min="15" max="15" width="37.85546875" style="28" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="28" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="37.85546875" style="28" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="28" customWidth="1"/>
     <col min="17" max="17" width="20.42578125" style="28" customWidth="1"/>
     <col min="18" max="18" width="23" style="20" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20.7109375" style="20" bestFit="1" customWidth="1"/>
@@ -1423,81 +1453,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="21" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="36"/>
+      <c r="N1" s="40"/>
       <c r="O1" s="30" t="s">
         <v>109</v>
       </c>
       <c r="P1" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="38" t="s">
+      <c r="Q1" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="40" t="s">
+      <c r="R1" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="38" t="s">
+      <c r="S1" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="38" t="s">
+      <c r="U1" s="31" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="33"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="37"/>
       <c r="M2" s="8" t="s">
         <v>90</v>
       </c>
@@ -1506,11 +1536,11 @@
       </c>
       <c r="O2" s="30"/>
       <c r="P2" s="30"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="38"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="31"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1570,7 +1600,7 @@
       <c r="U3" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="V3" s="41" t="s">
+      <c r="V3" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -1632,7 +1662,7 @@
       <c r="U4" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="V4" s="41" t="s">
+      <c r="V4" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -1694,7 +1724,7 @@
       <c r="U5" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="V5" s="41" t="s">
+      <c r="V5" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -1746,6 +1776,7 @@
       <c r="U6" s="10" t="s">
         <v>132</v>
       </c>
+      <c r="V6" s="14"/>
     </row>
     <row r="7" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1799,6 +1830,7 @@
       <c r="U7" s="10" t="s">
         <v>132</v>
       </c>
+      <c r="V7" s="14"/>
     </row>
     <row r="8" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1858,7 +1890,7 @@
       <c r="U8" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="V8" s="41" t="s">
+      <c r="V8" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -1920,7 +1952,7 @@
       <c r="U9" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="V9" s="41" t="s">
+      <c r="V9" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -1982,7 +2014,7 @@
       <c r="U10" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="V10" s="41" t="s">
+      <c r="V10" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2034,6 +2066,7 @@
       <c r="U11" s="10" t="s">
         <v>132</v>
       </c>
+      <c r="V11" s="14"/>
     </row>
     <row r="12" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -2083,6 +2116,7 @@
       <c r="U12" s="10" t="s">
         <v>132</v>
       </c>
+      <c r="V12" s="14"/>
     </row>
     <row r="13" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -2130,6 +2164,7 @@
       <c r="U13" s="10" t="s">
         <v>132</v>
       </c>
+      <c r="V13" s="14"/>
     </row>
     <row r="14" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -2189,7 +2224,7 @@
       <c r="U14" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="V14" s="41" t="s">
+      <c r="V14" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2245,65 +2280,67 @@
       <c r="U15" s="10" t="s">
         <v>132</v>
       </c>
+      <c r="V15" s="14"/>
     </row>
     <row r="16" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="22" t="s">
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="45">
         <v>14</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="J16" s="24" t="s">
+      <c r="J16" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="K16" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="L16" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7" t="s">
+      <c r="M16" s="42"/>
+      <c r="N16" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="O16" s="25" t="s">
+      <c r="O16" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="P16" s="26" t="s">
+      <c r="P16" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="Q16" s="10">
+      <c r="Q16" s="43">
         <v>6</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="R16" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="S16" s="10" t="s">
+      <c r="S16" s="43" t="s">
         <v>202</v>
       </c>
-      <c r="T16" s="12" t="s">
+      <c r="T16" s="47" t="s">
         <v>239</v>
       </c>
-      <c r="U16" s="10" t="s">
+      <c r="U16" s="43" t="s">
         <v>204</v>
       </c>
+      <c r="V16" s="43"/>
     </row>
     <row r="17" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -2359,6 +2396,7 @@
       <c r="U17" s="10" t="s">
         <v>132</v>
       </c>
+      <c r="V17" s="14"/>
     </row>
     <row r="18" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -2408,67 +2446,69 @@
       <c r="U18" s="10" t="s">
         <v>132</v>
       </c>
+      <c r="V18" s="14"/>
     </row>
     <row r="19" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="22" t="s">
+      <c r="F19" s="43"/>
+      <c r="G19" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="45">
         <v>17</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="J19" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="K19" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="M19" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="N19" s="7"/>
-      <c r="O19" s="25" t="s">
+      <c r="N19" s="42"/>
+      <c r="O19" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="P19" s="26" t="s">
+      <c r="P19" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="Q19" s="10">
+      <c r="Q19" s="43">
         <v>6</v>
       </c>
-      <c r="R19" s="11" t="s">
+      <c r="R19" s="43" t="s">
         <v>196</v>
       </c>
-      <c r="S19" s="10" t="s">
+      <c r="S19" s="43" t="s">
         <v>197</v>
       </c>
-      <c r="T19" s="12" t="s">
+      <c r="T19" s="47" t="s">
         <v>220</v>
       </c>
-      <c r="U19" s="10" t="s">
+      <c r="U19" s="43" t="s">
         <v>199</v>
       </c>
+      <c r="V19" s="43"/>
     </row>
     <row r="20" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -2526,6 +2566,7 @@
       <c r="U20" s="10" t="s">
         <v>132</v>
       </c>
+      <c r="V20" s="14"/>
     </row>
     <row r="21" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -2583,6 +2624,7 @@
       <c r="U21" s="10" t="s">
         <v>132</v>
       </c>
+      <c r="V21" s="14"/>
     </row>
     <row r="22" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -2642,7 +2684,7 @@
       <c r="U22" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="V22" s="41" t="s">
+      <c r="V22" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2692,6 +2734,7 @@
       <c r="U23" s="10" t="s">
         <v>132</v>
       </c>
+      <c r="V23" s="14"/>
     </row>
     <row r="24" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -2741,6 +2784,7 @@
       <c r="U24" s="10" t="s">
         <v>132</v>
       </c>
+      <c r="V24" s="14"/>
     </row>
     <row r="25" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -2800,7 +2844,7 @@
       <c r="U25" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="V25" s="41" t="s">
+      <c r="V25" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2862,7 +2906,7 @@
       <c r="U26" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="V26" s="41" t="s">
+      <c r="V26" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2918,7 +2962,7 @@
       <c r="U27" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="V27" s="41" t="s">
+      <c r="V27" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2980,7 +3024,7 @@
       <c r="U28" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="V28" s="41" t="s">
+      <c r="V28" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3042,7 +3086,7 @@
       <c r="U29" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="V29" s="41" t="s">
+      <c r="V29" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3098,7 +3142,7 @@
       <c r="U30" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="V30" s="41" t="s">
+      <c r="V30" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3148,7 +3192,7 @@
       <c r="U31" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="V31" s="41" t="s">
+      <c r="V31" s="29" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3210,11 +3254,11 @@
       <c r="U32" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="V32" s="41" t="s">
+      <c r="V32" s="29" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>15</v>
       </c>
@@ -3262,8 +3306,9 @@
       <c r="U33" s="10" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V33" s="14"/>
+    </row>
+    <row r="34" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>15</v>
       </c>
@@ -3311,8 +3356,9 @@
       <c r="U34" s="10" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V34" s="14"/>
+    </row>
+    <row r="35" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>15</v>
       </c>
@@ -3353,60 +3399,61 @@
       <c r="T35" s="12"/>
       <c r="U35" s="10"/>
     </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="43" t="s">
         <v>251</v>
       </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="16" t="s">
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="H36" s="23">
+      <c r="H36" s="45">
         <v>34</v>
       </c>
-      <c r="I36" s="14" t="s">
+      <c r="I36" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="J36" s="24" t="s">
+      <c r="J36" s="42" t="s">
         <v>194</v>
       </c>
-      <c r="K36" s="6" t="s">
+      <c r="K36" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="L36" s="5"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7" t="s">
+      <c r="L36" s="42"/>
+      <c r="M36" s="42"/>
+      <c r="N36" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="O36" s="25"/>
-      <c r="P36" s="26"/>
-      <c r="Q36" s="10">
+      <c r="O36" s="46"/>
+      <c r="P36" s="43"/>
+      <c r="Q36" s="43">
         <v>6</v>
       </c>
-      <c r="R36" s="11" t="s">
+      <c r="R36" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="S36" s="10" t="s">
+      <c r="S36" s="43" t="s">
         <v>202</v>
       </c>
-      <c r="T36" s="12" t="s">
+      <c r="T36" s="47" t="s">
         <v>245</v>
       </c>
-      <c r="U36" s="10" t="s">
+      <c r="U36" s="43" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V36" s="43"/>
+    </row>
+    <row r="37" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>15</v>
       </c>
@@ -3450,8 +3497,9 @@
       <c r="U37" s="10" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V37" s="14"/>
+    </row>
+    <row r="38" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="13"/>
       <c r="C38" s="9"/>
@@ -3474,7 +3522,7 @@
       <c r="T38" s="15"/>
       <c r="U38" s="10"/>
     </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="13"/>
       <c r="C39" s="9"/>
@@ -3497,7 +3545,7 @@
       <c r="T39" s="15"/>
       <c r="U39" s="10"/>
     </row>
-    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="13"/>
       <c r="C40" s="9"/>
@@ -3520,7 +3568,7 @@
       <c r="T40" s="15"/>
       <c r="U40" s="10"/>
     </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="13"/>
       <c r="C41" s="9"/>
@@ -3543,7 +3591,7 @@
       <c r="T41" s="15"/>
       <c r="U41" s="10"/>
     </row>
-    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="13"/>
       <c r="C42" s="9"/>
@@ -3566,7 +3614,7 @@
       <c r="T42" s="15"/>
       <c r="U42" s="10"/>
     </row>
-    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="13"/>
       <c r="C43" s="9"/>
@@ -3589,7 +3637,7 @@
       <c r="T43" s="15"/>
       <c r="U43" s="10"/>
     </row>
-    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="13"/>
       <c r="C44" s="9"/>
@@ -3612,7 +3660,7 @@
       <c r="T44" s="15"/>
       <c r="U44" s="10"/>
     </row>
-    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="13"/>
       <c r="C45" s="9"/>
@@ -3635,7 +3683,7 @@
       <c r="T45" s="15"/>
       <c r="U45" s="10"/>
     </row>
-    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="13"/>
       <c r="C46" s="9"/>
@@ -3658,7 +3706,7 @@
       <c r="T46" s="15"/>
       <c r="U46" s="10"/>
     </row>
-    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="13"/>
       <c r="C47" s="9"/>
@@ -3681,7 +3729,7 @@
       <c r="T47" s="15"/>
       <c r="U47" s="10"/>
     </row>
-    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="13"/>
       <c r="C48" s="9"/>
@@ -4585,12 +4633,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4605,6 +4647,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K37 L30:L37 L23:L24">

</xml_diff>